<commit_message>
Updated Bug metrics according to today's coding session
Updated Bug Metrics for todays coding session
1. Course DAO retrieve($course)
2. Prereq DAO retrieve($course)

Co-Authored-By: one-ice <one-ice@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43C440-B05A-4DA8-A003-E331035B4F51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D769890-8B1F-46BC-BD61-E278DDBAE34E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
   <si>
     <t>Bug Log</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>Retreive output table is not aligned properly</t>
+  </si>
+  <si>
+    <t>retrieve($course) in course DAO</t>
+  </si>
+  <si>
+    <t>retrieve($course) in Prerequisite DAO</t>
+  </si>
+  <si>
+    <t>Not all data was called in the select statement which made it impossible to create course objects. Results were also not appended in an array.</t>
+  </si>
+  <si>
+    <t>Not all data was called in the select statement which made it impossible to create prereq object. Results were also not appended in an array.</t>
   </si>
 </sst>
 </file>
@@ -472,9 +484,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -482,6 +491,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,7 +1121,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1126,16 +1138,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -1163,7 +1175,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -1171,21 +1183,38 @@
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+        <v>68</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="21">
+        <v>5</v>
+      </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
       <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="C4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="21">
+        <v>5</v>
+      </c>
       <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1432,7 +1461,7 @@
       <c r="B30" s="27"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21" t="str">
-        <f t="shared" ref="F3:F200" si="0">IF($E30="Critical", 10, IF($E30="High",5, IF($E30="Low",1,"")))</f>
+        <f t="shared" ref="F30:F200" si="0">IF($E30="Critical", 10, IF($E30="High",5, IF($E30="Low",1,"")))</f>
         <v/>
       </c>
     </row>
@@ -6546,16 +6575,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -6594,7 +6623,7 @@
       </c>
       <c r="C3" s="9" t="str">
         <f>'Our Bug Metrics'!$C3</f>
-        <v>Bootstrap</v>
+        <v>retrieve($course) in course DAO</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
@@ -16755,16 +16784,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -16812,7 +16841,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="34">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -16841,7 +16870,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -16864,7 +16893,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="31"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -16887,7 +16916,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -16910,7 +16939,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="31"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -16933,7 +16962,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -16956,7 +16985,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="34">
         <f>SUM(F9:F15)</f>
         <v>20</v>
       </c>
@@ -16985,7 +17014,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="31"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17008,7 +17037,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17031,7 +17060,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17054,7 +17083,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17077,7 +17106,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="34"/>
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17100,7 +17129,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -17123,7 +17152,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="34">
         <f>SUM(F16:F19)</f>
         <v>20</v>
       </c>
@@ -17152,7 +17181,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17175,7 +17204,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17198,7 +17227,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -17221,7 +17250,7 @@
         <f>IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="34">
         <f>SUM(F20:F23)</f>
         <v>12</v>
       </c>
@@ -17249,7 +17278,7 @@
       <c r="F21" s="28">
         <v>5</v>
       </c>
-      <c r="G21" s="31"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17272,7 +17301,7 @@
         <f>IF($E22="Critical", 10, IF($E22="High",5, IF($E22="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17295,7 +17324,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="31"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -22460,16 +22489,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -22508,11 +22537,11 @@
       </c>
       <c r="C3" s="9" t="str">
         <f>'Our Bug Metrics'!$C3</f>
-        <v>Bootstrap</v>
-      </c>
-      <c r="D3" s="10">
+        <v>retrieve($course) in course DAO</v>
+      </c>
+      <c r="D3" s="10" t="str">
         <f>'Our Bug Metrics'!$D3</f>
-        <v>0</v>
+        <v>Not all data was called in the select statement which made it impossible to create course objects. Results were also not appended in an array.</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>26</v>
@@ -22536,13 +22565,13 @@
         <f>'Our Bug Metrics'!$B4</f>
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="9" t="str">
         <f>'Our Bug Metrics'!$C4</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
+        <v>retrieve($course) in Prerequisite DAO</v>
+      </c>
+      <c r="D4" s="10" t="str">
         <f>'Our Bug Metrics'!$D4</f>
-        <v>0</v>
+        <v>Not all data was called in the select statement which made it impossible to create prereq object. Results were also not appended in an array.</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>26</v>
@@ -22587,7 +22616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <f>'Our Bug Metrics'!$A6</f>
         <v>4</v>
@@ -22613,7 +22642,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f>'Our Bug Metrics'!$A7</f>
         <v>5</v>

</xml_diff>

<commit_message>
Updated Bm.xlsx according to today's coding session
Co-Authored-By: Leonard Wong <leothelion96@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D769890-8B1F-46BC-BD61-E278DDBAE34E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E61E9-C8F7-4A9A-92E4-47AA9881BCEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="74">
   <si>
     <t>Bug Log</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Not all data was called in the select statement which made it impossible to create prereq object. Results were also not appended in an array.</t>
+  </si>
+  <si>
+    <t>Spelling error in function name.</t>
+  </si>
+  <si>
+    <t>Not all data was appended and returned in the results array.</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1217,28 +1223,46 @@
       </c>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3</v>
       </c>
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
       <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="C6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="21">
+        <v>5</v>
+      </c>
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -22526,7 +22550,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <f>'Our Bug Metrics'!$A3</f>
         <v>1</v>
@@ -22556,7 +22580,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <f>'Our Bug Metrics'!$A4</f>
         <v>2</v>
@@ -22595,13 +22619,13 @@
         <f>'Our Bug Metrics'!$B5</f>
         <v>1</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="9" t="str">
         <f>'Our Bug Metrics'!$C5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="10">
+        <v>retrieve($course) in Prerequisite DAO</v>
+      </c>
+      <c r="D5" s="10" t="str">
         <f>'Our Bug Metrics'!$D5</f>
-        <v>0</v>
+        <v>Spelling error in function name.</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>26</v>
@@ -22625,13 +22649,13 @@
         <f>'Our Bug Metrics'!$B6</f>
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="9" t="str">
         <f>'Our Bug Metrics'!$C6</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="10">
+        <v>retrieve($course) in Prerequisite DAO</v>
+      </c>
+      <c r="D6" s="10" t="str">
         <f>'Our Bug Metrics'!$D6</f>
-        <v>0</v>
+        <v>Not all data was appended and returned in the results array.</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated testcases and bug metrics to reflect testing for round 1 clearing
Updated testcases and bug metrics to reflect testing for round 1 clearing
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864D7F19-4671-44E6-917A-D8EB2185D2BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581657F3-AF41-40A4-B2B5-BBC565F61A33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="84">
   <si>
     <t>Bug Log</t>
   </si>
@@ -275,6 +275,15 @@
   <si>
     <t>YB &amp; SA</t>
   </si>
+  <si>
+    <t>Round 1 Clearing</t>
+  </si>
+  <si>
+    <t>Sectionstudent table contained all the bids who passed and failed instead of only passes after round 1 clearing.</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
 </sst>
 </file>
 
@@ -426,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -541,6 +550,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1698,15 +1710,31 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="23"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="24">
+        <v>2</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="18">
+        <v>5</v>
+      </c>
+      <c r="G17" s="19">
+        <v>5</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
@@ -6953,8 +6981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7393,7 +7421,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <f>'Our Bug Metrics'!$A16</f>
         <v>14</v>
@@ -7401,11 +7429,13 @@
       <c r="B16" s="8">
         <v>2</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>79</v>
+      <c r="C16" s="30" t="str">
+        <f>'Our Bug Metrics'!$C16</f>
+        <v>Add Bid</v>
+      </c>
+      <c r="D16" s="41" t="str">
+        <f>'Our Bug Metrics'!$D16</f>
+        <v>Variable names in course class differs from bidhome.php</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>26</v>
@@ -7420,31 +7450,46 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="17"/>
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
+        <f>'Our Bug Metrics'!$A17</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="30" t="str">
+        <f>'Our Bug Metrics'!$C17</f>
+        <v>Round 1 Clearing</v>
+      </c>
+      <c r="D17" s="31" t="str">
+        <f>'Our Bug Metrics'!$D17</f>
+        <v>Sectionstudent table contained all the bids who passed and failed instead of only passes after round 1 clearing.</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="17">
+        <v>43565</v>
+      </c>
       <c r="G17" s="17"/>
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="8"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="10"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="8"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="10"/>
       <c r="F19" s="17"/>
       <c r="G19" s="12"/>

</xml_diff>

<commit_message>
Updated Testcases and BM
Updated Testcases and BM to edit wrong entry
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581657F3-AF41-40A4-B2B5-BBC565F61A33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B0CF7F-9EDA-4868-AEBE-4C1F89492F9A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
   <si>
     <t>Bug Log</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>Sectionstudent table contained all the bids who passed and failed instead of only passes after round 1 clearing.</t>
-  </si>
-  <si>
-    <t>Unresolved</t>
   </si>
 </sst>
 </file>
@@ -541,6 +538,9 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,9 +550,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1309,16 +1306,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -6982,7 +6979,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6999,16 +6996,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -7433,7 +7430,7 @@
         <f>'Our Bug Metrics'!$C16</f>
         <v>Add Bid</v>
       </c>
-      <c r="D16" s="41" t="str">
+      <c r="D16" s="37" t="str">
         <f>'Our Bug Metrics'!$D16</f>
         <v>Variable names in course class differs from bidhome.php</v>
       </c>
@@ -7450,28 +7447,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
-        <f>'Our Bug Metrics'!$A17</f>
-        <v>15</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
-      <c r="C17" s="30" t="str">
-        <f>'Our Bug Metrics'!$C17</f>
-        <v>Round 1 Clearing</v>
-      </c>
-      <c r="D17" s="31" t="str">
-        <f>'Our Bug Metrics'!$D17</f>
-        <v>Sectionstudent table contained all the bids who passed and failed instead of only passes after round 1 clearing.</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="17">
-        <v>43565</v>
-      </c>
+    <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="16"/>
     </row>
@@ -17505,16 +17487,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -17562,7 +17544,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="41">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -17591,7 +17573,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17614,7 +17596,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -17637,7 +17619,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="40"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17660,7 +17642,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="40"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -17683,7 +17665,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="40"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -17706,7 +17688,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="41">
         <f>SUM(F9:F15)</f>
         <v>20</v>
       </c>
@@ -17735,7 +17717,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="40"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17758,7 +17740,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="40"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17781,7 +17763,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="40"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17804,7 +17786,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17827,7 +17809,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="40"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17850,7 +17832,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -17873,7 +17855,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="41">
         <f>SUM(F16:F19)</f>
         <v>20</v>
       </c>
@@ -17902,7 +17884,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="40"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17925,7 +17907,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="40"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17948,7 +17930,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="40"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -17971,7 +17953,7 @@
         <f>IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="41">
         <f>SUM(F20:F23)</f>
         <v>12</v>
       </c>
@@ -17999,7 +17981,7 @@
       <c r="F21" s="25">
         <v>5</v>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18022,7 +18004,7 @@
         <f>IF($E22="Critical", 10, IF($E22="High",5, IF($E22="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G22" s="40"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18045,7 +18027,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="41"/>
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated BM to reflect latest bugs
Updated BM to reflect latest bugs

Co-Authored-By: tohjaslyn <tohjaslyn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418A9392-00ED-439C-8142-476CB124B8D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCE74DB-51E8-49B9-A5DF-232854613569}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="100">
   <si>
     <t>Bug Log</t>
   </si>
@@ -329,6 +329,9 @@
   <si>
     <t>bidding.php shows error as did not code what to display if there are no sections available.</t>
   </si>
+  <si>
+    <t>bid table not cleared during clearing</t>
+  </si>
 </sst>
 </file>
 
@@ -480,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -589,6 +592,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,59 +609,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="55">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -894,6 +848,89 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1388,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:H23"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1406,16 +1443,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -1993,18 +2030,34 @@
       <c r="A24" s="18">
         <v>22</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="23"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="str">
+      <c r="B24" s="24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="18">
         <f>IF($E24="Critical", 10, IF($E24="High",5, IF($E24="Low",1,"")))</f>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="19">
+        <v>1</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>23</v>
       </c>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
@@ -7111,59 +7164,64 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H2 H12:H21 H24:H1048576">
-    <cfRule type="containsText" dxfId="50" priority="23" operator="containsText" text="Stop current Development">
+  <conditionalFormatting sqref="H1:H2 H12:H21 H26:H1048576">
+    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="49" priority="22" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="53" priority="23" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="48" priority="16" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="52" priority="17" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="51" priority="15" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="45" priority="9" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="49" priority="10" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="48" priority="9" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H23">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="Stop current Development">
+      <formula>NOT(ISERROR(SEARCH("Stop current Development",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7179,8 +7237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7197,16 +7255,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -7847,10 +7905,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="17">
-        <v>43687</v>
+        <v>43746</v>
       </c>
       <c r="G24" s="17">
-        <v>43687</v>
+        <v>43746</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>80</v>
@@ -7873,24 +7931,40 @@
         <v>26</v>
       </c>
       <c r="F25" s="17">
-        <v>43687</v>
+        <v>43746</v>
       </c>
       <c r="G25" s="17">
-        <v>43687</v>
+        <v>43746</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="11"/>
+    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8">
+        <v>2</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="12">
+        <v>43749</v>
+      </c>
+      <c r="G26" s="12">
+        <v>43750</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
@@ -17637,202 +17711,217 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="40" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="39" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="containsBlanks" dxfId="38" priority="51">
+    <cfRule type="containsBlanks" dxfId="40" priority="54">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsBlanks" dxfId="35" priority="36">
+    <cfRule type="containsBlanks" dxfId="37" priority="39">
       <formula>LEN(TRIM(E10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsBlanks" dxfId="32" priority="33">
+    <cfRule type="containsBlanks" dxfId="34" priority="36">
       <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsBlanks" dxfId="29" priority="30">
+    <cfRule type="containsBlanks" dxfId="31" priority="33">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsBlanks" dxfId="26" priority="27">
+    <cfRule type="containsBlanks" dxfId="28" priority="30">
       <formula>LEN(TRIM(E8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsBlanks" dxfId="23" priority="24">
+    <cfRule type="containsBlanks" dxfId="25" priority="27">
       <formula>LEN(TRIM(E7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="20" priority="21">
+    <cfRule type="containsBlanks" dxfId="22" priority="24">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsBlanks" dxfId="17" priority="18">
+    <cfRule type="containsBlanks" dxfId="19" priority="21">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="14" priority="15">
+    <cfRule type="containsBlanks" dxfId="16" priority="18">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(E24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
+      <formula>LEN(TRIM(E26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E25" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E26" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17862,16 +17951,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -17919,7 +18008,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="42">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -17948,7 +18037,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -17971,7 +18060,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -17994,7 +18083,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18017,7 +18106,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -18040,7 +18129,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -18063,7 +18152,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="42">
         <f>SUM(F9:F15)</f>
         <v>20</v>
       </c>
@@ -18092,7 +18181,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18115,7 +18204,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18138,7 +18227,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="41"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18161,7 +18250,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18184,7 +18273,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18207,7 +18296,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -18230,7 +18319,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="42">
         <f>SUM(F16:F19)</f>
         <v>20</v>
       </c>
@@ -18259,7 +18348,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18282,7 +18371,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="41"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18305,7 +18394,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="41"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -18328,7 +18417,7 @@
         <f>IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G20" s="41">
+      <c r="G20" s="42">
         <f>SUM(F20:F23)</f>
         <v>12</v>
       </c>
@@ -18356,7 +18445,7 @@
       <c r="F21" s="25">
         <v>5</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18379,7 +18468,7 @@
         <f>IF($E22="Critical", 10, IF($E22="High",5, IF($E22="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G22" s="41"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -18402,7 +18491,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="41"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -23532,7 +23621,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/SMU-IS212/project-g5t4"
This reverts commit 6f7e60a178b897324164f82b70a73305ed5573f4, reversing
changes made to d07ea505b61a644bb8a36de7c667828ec73cc599.
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CABB2C-B308-41D9-A6FC-59FFA5808C24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A6E536-6CC5-49BF-85D5-B848A1F7638D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="144">
   <si>
     <t>Bug Log</t>
   </si>
@@ -402,6 +402,9 @@
     <t>For a section vacancy of 2 in IS003 S1, 2 students first bid $10. Then, a third person bids $11 but the original 2 were not kicked out of the section</t>
   </si>
   <si>
+    <t>Unresolved</t>
+  </si>
+  <si>
     <t>SH &amp; LW</t>
   </si>
   <si>
@@ -763,16 +766,6 @@
   </cellStyles>
   <dxfs count="103">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none"/>
       </fill>
@@ -811,6 +804,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1949,7 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -19379,10 +19382,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E41" s="40" t="s">
         <v>38</v>
@@ -19406,10 +19409,10 @@
         <v>4</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E42" s="40" t="s">
         <v>31</v>
@@ -19432,10 +19435,10 @@
         <v>4</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E43" s="43" t="s">
         <v>31</v>
@@ -19459,10 +19462,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E44" s="40" t="s">
         <v>31</v>
@@ -19486,10 +19489,10 @@
         <v>4</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E45" s="40" t="s">
         <v>31</v>
@@ -19513,10 +19516,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>31</v>
@@ -19540,10 +19543,10 @@
         <v>4</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E47" s="40" t="s">
         <v>31</v>
@@ -19567,10 +19570,10 @@
         <v>4</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E48" s="40" t="s">
         <v>31</v>
@@ -19596,7 +19599,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E49" s="40" t="s">
         <v>31</v>
@@ -19620,10 +19623,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>31</v>
@@ -19646,10 +19649,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>31</v>
@@ -19672,10 +19675,10 @@
         <v>4</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>31</v>
@@ -24527,8 +24530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25665,16 +25668,14 @@
         <v>For a section vacancy of 2 in IS003 S1, 2 students first bid $10. Then, a third person bids $11 but the original 2 were not kicked out of the section</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="F40" s="12">
         <v>43774</v>
       </c>
-      <c r="G40" s="12">
-        <v>43775</v>
-      </c>
+      <c r="G40" s="12"/>
       <c r="H40" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -25704,7 +25705,7 @@
         <v>43768</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -25734,7 +25735,7 @@
         <v>43769</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25764,7 +25765,7 @@
         <v>43769</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25794,7 +25795,7 @@
         <v>43769</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25824,7 +25825,7 @@
         <v>43769</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25854,7 +25855,7 @@
         <v>43769</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25884,7 +25885,7 @@
         <v>43769</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25914,7 +25915,7 @@
         <v>43769</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25944,7 +25945,7 @@
         <v>43775</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25974,7 +25975,7 @@
         <v>43775</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25987,10 +25988,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>26</v>
@@ -26002,7 +26003,7 @@
         <v>43775</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -26032,7 +26033,7 @@
         <v>43775</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -35977,32 +35978,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41708,7 +41709,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/SMU-IS212/project-g5t4""
This reverts commit a69cb230d374507df67d174afc249b62f194c33c.
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A6E536-6CC5-49BF-85D5-B848A1F7638D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CABB2C-B308-41D9-A6FC-59FFA5808C24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="143">
   <si>
     <t>Bug Log</t>
   </si>
@@ -402,9 +402,6 @@
     <t>For a section vacancy of 2 in IS003 S1, 2 students first bid $10. Then, a third person bids $11 but the original 2 were not kicked out of the section</t>
   </si>
   <si>
-    <t>Unresolved</t>
-  </si>
-  <si>
     <t>SH &amp; LW</t>
   </si>
   <si>
@@ -766,6 +763,16 @@
   </cellStyles>
   <dxfs count="103">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none"/>
       </fill>
@@ -804,16 +811,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1952,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -19382,10 +19379,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>126</v>
       </c>
       <c r="E41" s="40" t="s">
         <v>38</v>
@@ -19409,10 +19406,10 @@
         <v>4</v>
       </c>
       <c r="C42" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="E42" s="40" t="s">
         <v>31</v>
@@ -19435,10 +19432,10 @@
         <v>4</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E43" s="43" t="s">
         <v>31</v>
@@ -19462,10 +19459,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E44" s="40" t="s">
         <v>31</v>
@@ -19489,10 +19486,10 @@
         <v>4</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E45" s="40" t="s">
         <v>31</v>
@@ -19516,10 +19513,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>31</v>
@@ -19543,10 +19540,10 @@
         <v>4</v>
       </c>
       <c r="C47" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="22" t="s">
         <v>133</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>134</v>
       </c>
       <c r="E47" s="40" t="s">
         <v>31</v>
@@ -19570,10 +19567,10 @@
         <v>4</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48" s="40" t="s">
         <v>31</v>
@@ -19599,7 +19596,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E49" s="40" t="s">
         <v>31</v>
@@ -19623,10 +19620,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="22" t="s">
         <v>137</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>138</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>31</v>
@@ -19649,10 +19646,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>31</v>
@@ -19675,10 +19672,10 @@
         <v>4</v>
       </c>
       <c r="C52" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>31</v>
@@ -24530,8 +24527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25668,14 +25665,16 @@
         <v>For a section vacancy of 2 in IS003 S1, 2 students first bid $10. Then, a third person bids $11 but the original 2 were not kicked out of the section</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="F40" s="12">
         <v>43774</v>
       </c>
-      <c r="G40" s="12"/>
+      <c r="G40" s="12">
+        <v>43775</v>
+      </c>
       <c r="H40" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -25705,7 +25704,7 @@
         <v>43768</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -25735,7 +25734,7 @@
         <v>43769</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25765,7 +25764,7 @@
         <v>43769</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25795,7 +25794,7 @@
         <v>43769</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25825,7 +25824,7 @@
         <v>43769</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25855,7 +25854,7 @@
         <v>43769</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25885,7 +25884,7 @@
         <v>43769</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25915,7 +25914,7 @@
         <v>43769</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25945,7 +25944,7 @@
         <v>43775</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25975,7 +25974,7 @@
         <v>43775</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -25988,10 +25987,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>26</v>
@@ -26003,7 +26002,7 @@
         <v>43775</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -26033,7 +26032,7 @@
         <v>43775</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -35978,32 +35977,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41709,7 +41708,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated BM for Section dump using UAT json test
Updated BM for Section dump using UAT json test
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CABB2C-B308-41D9-A6FC-59FFA5808C24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E7EF4F-EAC2-4948-A383-99A0B9FD771C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="145">
   <si>
     <t>Bug Log</t>
   </si>
@@ -461,6 +461,12 @@
   <si>
     <t>JSON output includes round 1 successful bids</t>
   </si>
+  <si>
+    <t>section-dump.php</t>
+  </si>
+  <si>
+    <t>JSON output indicates NULL for student instead of empty array</t>
+  </si>
 </sst>
 </file>
 
@@ -761,7 +767,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="106">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -769,6 +775,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1949,8 +1976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A38" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19694,10 +19721,27 @@
       <c r="A53" s="43">
         <v>51</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="F53" s="40" t="str">
+      <c r="B53" s="24">
+        <v>4</v>
+      </c>
+      <c r="C53" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="40">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G53" s="40">
+        <v>1</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -24395,122 +24439,122 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2 H12:H21 H37:H39 H42:H1048576">
-    <cfRule type="containsText" dxfId="102" priority="39" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="105" priority="39" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="101" priority="38" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="104" priority="38" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="100" priority="32" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="103" priority="32" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="99" priority="30" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="102" priority="30" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="98" priority="26" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="101" priority="26" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="97" priority="25" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="100" priority="25" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="96" priority="24" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="99" priority="24" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="95" priority="20" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="98" priority="20" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="94" priority="19" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="97" priority="19" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="93" priority="18" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="96" priority="18" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="92" priority="17" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="95" priority="17" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="91" priority="15" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="94" priority="15" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="89" priority="11" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="92" priority="11" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="88" priority="10" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="91" priority="10" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="90" priority="9" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="86" priority="8" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="89" priority="8" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="85" priority="7" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="88" priority="7" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="83" priority="5" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="82" priority="4" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="85" priority="4" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H36">
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="84" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="83" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="79" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H41)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24528,7 +24572,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26042,20 +26086,28 @@
       </c>
       <c r="B53" s="30">
         <f>'Our Bug Metrics'!B53</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="30">
+        <v>4</v>
+      </c>
+      <c r="C53" s="30" t="str">
         <f>'Our Bug Metrics'!C53</f>
-        <v>0</v>
-      </c>
-      <c r="D53" s="15">
+        <v>section-dump.php</v>
+      </c>
+      <c r="D53" s="15" t="str">
         <f>'Our Bug Metrics'!D53</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="11"/>
+        <v>JSON output indicates NULL for student instead of empty array</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="12">
+        <v>43781</v>
+      </c>
+      <c r="G53" s="12">
+        <v>43781</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
@@ -35617,397 +35669,412 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="78" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="94" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="77" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="95" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="containsBlanks" dxfId="76" priority="93">
+    <cfRule type="containsBlanks" dxfId="79" priority="96">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsBlanks" dxfId="76" priority="81">
+      <formula>LEN(TRIM(E10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
     <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="E11">
     <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="E11">
     <cfRule type="containsBlanks" dxfId="73" priority="78">
-      <formula>LEN(TRIM(E10))=0</formula>
+      <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="E9">
     <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="E9">
     <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="E9">
     <cfRule type="containsBlanks" dxfId="70" priority="75">
-      <formula>LEN(TRIM(E11))=0</formula>
+      <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="E8">
     <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="E8">
     <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="E8">
     <cfRule type="containsBlanks" dxfId="67" priority="72">
-      <formula>LEN(TRIM(E9))=0</formula>
+      <formula>LEN(TRIM(E8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E7">
     <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E7">
     <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E7">
     <cfRule type="containsBlanks" dxfId="64" priority="69">
-      <formula>LEN(TRIM(E8))=0</formula>
+      <formula>LEN(TRIM(E7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="E12">
     <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="E12">
     <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="E12">
     <cfRule type="containsBlanks" dxfId="61" priority="66">
-      <formula>LEN(TRIM(E7))=0</formula>
+      <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E6">
     <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E6">
     <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E6">
     <cfRule type="containsBlanks" dxfId="58" priority="63">
-      <formula>LEN(TRIM(E12))=0</formula>
+      <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="E21">
     <cfRule type="containsBlanks" dxfId="55" priority="60">
-      <formula>LEN(TRIM(E6))=0</formula>
+      <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="containsBlanks" dxfId="52" priority="57">
-      <formula>LEN(TRIM(E21))=0</formula>
+      <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E23">
     <cfRule type="containsBlanks" dxfId="49" priority="54">
-      <formula>LEN(TRIM(E22))=0</formula>
+      <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E24">
     <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E24">
     <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E24">
     <cfRule type="containsBlanks" dxfId="46" priority="51">
-      <formula>LEN(TRIM(E23))=0</formula>
+      <formula>LEN(TRIM(E24))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E25">
     <cfRule type="containsBlanks" dxfId="43" priority="48">
-      <formula>LEN(TRIM(E24))=0</formula>
+      <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E26:E27">
     <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E26:E27">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E26:E27">
     <cfRule type="containsBlanks" dxfId="40" priority="45">
-      <formula>LEN(TRIM(E25))=0</formula>
+      <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
+  <conditionalFormatting sqref="E28">
     <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
+  <conditionalFormatting sqref="E28">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
+  <conditionalFormatting sqref="E28">
     <cfRule type="containsBlanks" dxfId="37" priority="42">
-      <formula>LEN(TRIM(E26))=0</formula>
+      <formula>LEN(TRIM(E28))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E29">
     <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E29">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E29">
     <cfRule type="containsBlanks" dxfId="34" priority="39">
-      <formula>LEN(TRIM(E28))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
-      <formula>"Unresolved"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
-      <formula>"Resolved"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="containsBlanks" dxfId="31" priority="36">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="containsBlanks" dxfId="31" priority="33">
+      <formula>LEN(TRIM(E30))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E31">
     <cfRule type="containsBlanks" dxfId="28" priority="30">
-      <formula>LEN(TRIM(E30))=0</formula>
+      <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="containsBlanks" dxfId="25" priority="27">
-      <formula>LEN(TRIM(E31))=0</formula>
+      <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E33:E39">
     <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E33:E39">
     <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E33:E39">
     <cfRule type="containsBlanks" dxfId="22" priority="24">
-      <formula>LEN(TRIM(E32))=0</formula>
+      <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33:E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33:E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33:E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="containsBlanks" dxfId="19" priority="21">
-      <formula>LEN(TRIM(E33))=0</formula>
+      <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="containsBlanks" dxfId="16" priority="18">
-      <formula>LEN(TRIM(E40))=0</formula>
+      <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42:E48">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42:E48">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42:E48">
     <cfRule type="containsBlanks" dxfId="13" priority="15">
-      <formula>LEN(TRIM(E41))=0</formula>
+      <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E48">
+  <conditionalFormatting sqref="E49:E50">
     <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E48">
+  <conditionalFormatting sqref="E49:E50">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E48">
+  <conditionalFormatting sqref="E49:E50">
     <cfRule type="containsBlanks" dxfId="10" priority="12">
-      <formula>LEN(TRIM(E42))=0</formula>
+      <formula>LEN(TRIM(E49))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="containsBlanks" dxfId="7" priority="9">
-      <formula>LEN(TRIM(E49))=0</formula>
+      <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="containsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(E51))=0</formula>
+      <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(E52))=0</formula>
+      <formula>LEN(TRIM(E53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E52" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E53" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "Updated BM for Section dump using UAT json test"
This reverts commit 2bb65be48431a3db7328f35c2f7a1a22dbc74ae5.
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E7EF4F-EAC2-4948-A383-99A0B9FD771C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CABB2C-B308-41D9-A6FC-59FFA5808C24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="143">
   <si>
     <t>Bug Log</t>
   </si>
@@ -461,12 +461,6 @@
   <si>
     <t>JSON output includes round 1 successful bids</t>
   </si>
-  <si>
-    <t>section-dump.php</t>
-  </si>
-  <si>
-    <t>JSON output indicates NULL for student instead of empty array</t>
-  </si>
 </sst>
 </file>
 
@@ -767,7 +761,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="103">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -775,27 +769,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1976,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52:H53"/>
+    <sheetView topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19721,27 +19694,10 @@
       <c r="A53" s="43">
         <v>51</v>
       </c>
-      <c r="B53" s="24">
-        <v>4</v>
-      </c>
-      <c r="C53" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F53" s="40">
+      <c r="B53" s="24"/>
+      <c r="F53" s="40" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G53" s="40">
-        <v>1</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>64</v>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -24439,122 +24395,122 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2 H12:H21 H37:H39 H42:H1048576">
-    <cfRule type="containsText" dxfId="105" priority="39" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="102" priority="39" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="104" priority="38" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="101" priority="38" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="103" priority="32" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="100" priority="32" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="102" priority="30" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="99" priority="30" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="101" priority="26" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="98" priority="26" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="100" priority="25" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="97" priority="25" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="99" priority="24" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="96" priority="24" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="98" priority="20" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="95" priority="20" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="97" priority="19" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="94" priority="19" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="96" priority="18" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="93" priority="18" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="95" priority="17" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="92" priority="17" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="94" priority="15" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="91" priority="15" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="92" priority="11" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="89" priority="11" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="91" priority="10" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="88" priority="10" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="90" priority="9" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="89" priority="8" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="86" priority="8" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="88" priority="7" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="85" priority="7" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="83" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="85" priority="4" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="82" priority="4" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H36">
-    <cfRule type="containsText" dxfId="84" priority="3" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="83" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="79" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H41)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24572,7 +24528,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26086,28 +26042,20 @@
       </c>
       <c r="B53" s="30">
         <f>'Our Bug Metrics'!B53</f>
-        <v>4</v>
-      </c>
-      <c r="C53" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="C53" s="30">
         <f>'Our Bug Metrics'!C53</f>
-        <v>section-dump.php</v>
-      </c>
-      <c r="D53" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="D53" s="15">
         <f>'Our Bug Metrics'!D53</f>
-        <v>JSON output indicates NULL for student instead of empty array</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="12">
-        <v>43781</v>
-      </c>
-      <c r="G53" s="12">
-        <v>43781</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>123</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
@@ -35669,412 +35617,397 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="81" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="91" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="80" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="92" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="containsBlanks" dxfId="79" priority="96">
+    <cfRule type="containsBlanks" dxfId="76" priority="93">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsBlanks" dxfId="76" priority="81">
+    <cfRule type="containsBlanks" dxfId="73" priority="78">
       <formula>LEN(TRIM(E10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsBlanks" dxfId="73" priority="78">
+    <cfRule type="containsBlanks" dxfId="70" priority="75">
       <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsBlanks" dxfId="70" priority="75">
+    <cfRule type="containsBlanks" dxfId="67" priority="72">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsBlanks" dxfId="67" priority="72">
+    <cfRule type="containsBlanks" dxfId="64" priority="69">
       <formula>LEN(TRIM(E8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsBlanks" dxfId="64" priority="69">
+    <cfRule type="containsBlanks" dxfId="61" priority="66">
       <formula>LEN(TRIM(E7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="61" priority="66">
+    <cfRule type="containsBlanks" dxfId="58" priority="63">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsBlanks" dxfId="58" priority="63">
+    <cfRule type="containsBlanks" dxfId="55" priority="60">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="55" priority="60">
+    <cfRule type="containsBlanks" dxfId="52" priority="57">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="52" priority="57">
+    <cfRule type="containsBlanks" dxfId="49" priority="54">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="49" priority="54">
+    <cfRule type="containsBlanks" dxfId="46" priority="51">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="containsBlanks" dxfId="46" priority="51">
+    <cfRule type="containsBlanks" dxfId="43" priority="48">
       <formula>LEN(TRIM(E24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="containsBlanks" dxfId="43" priority="48">
+    <cfRule type="containsBlanks" dxfId="40" priority="45">
       <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsBlanks" dxfId="40" priority="45">
+    <cfRule type="containsBlanks" dxfId="37" priority="42">
       <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="containsBlanks" dxfId="37" priority="42">
+    <cfRule type="containsBlanks" dxfId="34" priority="39">
       <formula>LEN(TRIM(E28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="containsBlanks" dxfId="34" priority="39">
+    <cfRule type="containsBlanks" dxfId="31" priority="36">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="31" priority="33">
+    <cfRule type="containsBlanks" dxfId="28" priority="30">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsBlanks" dxfId="28" priority="30">
+    <cfRule type="containsBlanks" dxfId="25" priority="27">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsBlanks" dxfId="25" priority="27">
+    <cfRule type="containsBlanks" dxfId="22" priority="24">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="containsBlanks" dxfId="22" priority="24">
+    <cfRule type="containsBlanks" dxfId="19" priority="21">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsBlanks" dxfId="19" priority="21">
+    <cfRule type="containsBlanks" dxfId="16" priority="18">
       <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(E49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Unresolved"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Resolved"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(E53))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E53" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E52" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated BM to reflect bug in bootstrap
Updated BM to reflect bug in bootstrap
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F412092-198D-40A0-BD3D-904DDA3D4234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A5A46-9AB8-431F-9C19-A8F1E677B5EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="150">
   <si>
     <t>Bug Log</t>
   </si>
@@ -476,6 +476,12 @@
   <si>
     <t>Json shows Null when no students in section instead of empty array</t>
   </si>
+  <si>
+    <t xml:space="preserve">Student edollar is invalid when it is 1d.p. </t>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
 </sst>
 </file>
 
@@ -776,7 +782,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="113">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2006,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53:H54"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19800,14 +19837,31 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A55" s="43">
         <v>53</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="F55" s="40" t="str">
+      <c r="B55" s="24">
+        <v>5</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="40">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
+      </c>
+      <c r="G55" s="40">
+        <v>5</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -24484,124 +24538,129 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H2 H12:H21 H37:H39 H42:H1048576">
-    <cfRule type="containsText" dxfId="108" priority="39" operator="containsText" text="Stop current Development">
+  <conditionalFormatting sqref="H1:H2 H12:H21 H37:H39 H42:H54 H56:H1048576">
+    <cfRule type="containsText" dxfId="112" priority="40" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="107" priority="38" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="111" priority="39" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="106" priority="32" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="110" priority="33" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="105" priority="30" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="109" priority="31" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="104" priority="26" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="108" priority="27" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="103" priority="25" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="107" priority="26" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="102" priority="24" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="106" priority="25" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="101" priority="20" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="105" priority="21" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="100" priority="19" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="104" priority="20" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="99" priority="18" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="103" priority="19" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="98" priority="17" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="102" priority="18" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="97" priority="15" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="101" priority="16" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="100" priority="13" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="95" priority="11" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="99" priority="12" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="94" priority="10" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="98" priority="11" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="97" priority="10" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="92" priority="8" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="91" priority="7" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="95" priority="8" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="94" priority="7" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="89" priority="5" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="93" priority="6" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="88" priority="4" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="92" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H36">
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="91" priority="4" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H55">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Stop current Development">
+      <formula>NOT(ISERROR(SEARCH("Stop current Development",H55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -24617,8 +24676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A38" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26192,20 +26251,26 @@
       </c>
       <c r="B55" s="30">
         <f>'Our Bug Metrics'!B55</f>
-        <v>0</v>
-      </c>
-      <c r="C55" s="30">
+        <v>5</v>
+      </c>
+      <c r="C55" s="30" t="str">
         <f>'Our Bug Metrics'!C55</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="15">
+        <v>Bootstrap</v>
+      </c>
+      <c r="D55" s="15" t="str">
         <f>'Our Bug Metrics'!D55</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="12"/>
+        <v xml:space="preserve">Student edollar is invalid when it is 1d.p. </v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="12">
+        <v>43811</v>
+      </c>
       <c r="G55" s="12"/>
-      <c r="H55" s="11"/>
+      <c r="H55" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
@@ -35723,427 +35788,442 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="84" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="83" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="101" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="containsBlanks" dxfId="82" priority="99">
+    <cfRule type="containsBlanks" dxfId="86" priority="102">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="80" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="86" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsBlanks" dxfId="79" priority="84">
+    <cfRule type="containsBlanks" dxfId="83" priority="87">
       <formula>LEN(TRIM(E10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsBlanks" dxfId="76" priority="81">
+    <cfRule type="containsBlanks" dxfId="80" priority="84">
       <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="80" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsBlanks" dxfId="73" priority="78">
+    <cfRule type="containsBlanks" dxfId="77" priority="81">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="76" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="77" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsBlanks" dxfId="70" priority="75">
+    <cfRule type="containsBlanks" dxfId="74" priority="78">
       <formula>LEN(TRIM(E8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsBlanks" dxfId="67" priority="72">
+    <cfRule type="containsBlanks" dxfId="71" priority="75">
       <formula>LEN(TRIM(E7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="64" priority="69">
+    <cfRule type="containsBlanks" dxfId="68" priority="72">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsBlanks" dxfId="61" priority="66">
+    <cfRule type="containsBlanks" dxfId="65" priority="69">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="64" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="58" priority="63">
+    <cfRule type="containsBlanks" dxfId="62" priority="66">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="55" priority="60">
+    <cfRule type="containsBlanks" dxfId="59" priority="63">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="52" priority="57">
+    <cfRule type="containsBlanks" dxfId="56" priority="60">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="containsBlanks" dxfId="49" priority="54">
+    <cfRule type="containsBlanks" dxfId="53" priority="57">
       <formula>LEN(TRIM(E24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="containsBlanks" dxfId="46" priority="51">
+    <cfRule type="containsBlanks" dxfId="50" priority="54">
       <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsBlanks" dxfId="43" priority="48">
+    <cfRule type="containsBlanks" dxfId="47" priority="51">
       <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="containsBlanks" dxfId="40" priority="45">
+    <cfRule type="containsBlanks" dxfId="44" priority="48">
       <formula>LEN(TRIM(E28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="containsBlanks" dxfId="37" priority="42">
+    <cfRule type="containsBlanks" dxfId="41" priority="45">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="34" priority="36">
+    <cfRule type="containsBlanks" dxfId="38" priority="39">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsBlanks" dxfId="31" priority="33">
+    <cfRule type="containsBlanks" dxfId="35" priority="36">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsBlanks" dxfId="28" priority="30">
+    <cfRule type="containsBlanks" dxfId="32" priority="33">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="containsBlanks" dxfId="25" priority="27">
+    <cfRule type="containsBlanks" dxfId="29" priority="30">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsBlanks" dxfId="22" priority="24">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
       <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsBlanks" dxfId="19" priority="21">
+    <cfRule type="containsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
       <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(E49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(E53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(E54))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(E55))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E54" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E55" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>
@@ -41844,7 +41924,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update BM.xlsx to reflect the updated bugs
Update BM.xlsx to reflect the updated bugs
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DA9D4F-6FC2-4977-97CA-0F2BDE7FAA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D4D761-1282-4841-8CE0-A7358E4DE443}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="149">
   <si>
     <t>Bug Log</t>
   </si>
@@ -479,9 +479,6 @@
   <si>
     <t xml:space="preserve">Student edollar is invalid when it is 1d.p. </t>
   </si>
-  <si>
-    <t>Unresolved</t>
-  </si>
 </sst>
 </file>
 
@@ -790,6 +787,16 @@
   </cellStyles>
   <dxfs count="116">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none"/>
       </fill>
@@ -807,16 +814,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -24700,7 +24697,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26228,10 +26225,10 @@
         <v>26</v>
       </c>
       <c r="F53" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="G53" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="H53" s="16" t="s">
         <v>145</v>
@@ -26258,10 +26255,10 @@
         <v>26</v>
       </c>
       <c r="F54" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="G54" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>145</v>
@@ -26288,10 +26285,10 @@
         <v>26</v>
       </c>
       <c r="F55" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="G55" s="12">
-        <v>43810</v>
+        <v>43781</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>145</v>
@@ -26315,13 +26312,17 @@
         <v xml:space="preserve">Student edollar is invalid when it is 1d.p. </v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="F56" s="12">
-        <v>43810</v>
-      </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="11"/>
+        <v>43781</v>
+      </c>
+      <c r="G56" s="12">
+        <v>43782</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
@@ -36252,17 +36253,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(E56))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41968,7 +41969,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update BM.xlsx to reflect latest bug state
Update BM.xlsx to reflect latest bug state
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D4D761-1282-4841-8CE0-A7358E4DE443}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FA6711-DF49-4B57-A5C9-9F210080C99C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="151">
   <si>
     <t>Bug Log</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t xml:space="preserve">Student edollar is invalid when it is 1d.p. </t>
+  </si>
+  <si>
+    <t>Json Drop section</t>
+  </si>
+  <si>
+    <t>Incorrect error message in Json dropsection</t>
   </si>
 </sst>
 </file>
@@ -24696,8 +24702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25825,22 +25831,20 @@
         <f>'Our Bug Metrics'!B40</f>
         <v>0</v>
       </c>
-      <c r="C40" s="30">
-        <f>'Our Bug Metrics'!C40</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="15">
-        <f>'Our Bug Metrics'!D40</f>
-        <v>0</v>
+      <c r="C40" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="12">
-        <v>43774</v>
+        <v>43767</v>
       </c>
       <c r="G40" s="12">
-        <v>43775</v>
+        <v>43767</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Updated BM.xlsx due to error line in line 39
Updated BM.xlsx due to error line in line 39
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FA6711-DF49-4B57-A5C9-9F210080C99C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2BDAFD-033F-4D3E-91CC-75D94CEF93E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="151">
   <si>
     <t>Bug Log</t>
   </si>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19468,12 +19468,31 @@
       <c r="XFC39" s="30"/>
       <c r="XFD39" s="15"/>
     </row>
-    <row r="40" spans="1:16384" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16384" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="42">
         <v>38</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="H40" s="22"/>
+      <c r="B40" s="24">
+        <v>4</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="30">
+        <v>1</v>
+      </c>
+      <c r="G40" s="30">
+        <v>1</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="41" spans="1:16384" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A41" s="43">
@@ -24564,7 +24583,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H2 H12:H21 H37:H39 H42:H48 H50:H1048576">
+  <conditionalFormatting sqref="H1:H2 H12:H21 H42:H48 H50:H1048576 H37:H40">
     <cfRule type="containsText" dxfId="115" priority="40" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
@@ -24674,11 +24693,6 @@
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Stop current Development">
-      <formula>NOT(ISERROR(SEARCH("Stop current Development",H40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H41">
     <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H41)))</formula>
@@ -24702,8 +24716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="A28" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25828,8 +25842,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="30">
-        <f>'Our Bug Metrics'!B40</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
Updated BM.xlsx regarding bootstrap bug where section S01 is accepted
Updated BM.xlsx regarding bootstrap bug where section S01 is accepted

Co-Authored-By: serene98 <serene98@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2BDAFD-033F-4D3E-91CC-75D94CEF93E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ADD36E-B616-46AA-811C-26634C8666B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="152">
   <si>
     <t>Bug Log</t>
   </si>
@@ -485,6 +485,9 @@
   <si>
     <t>Incorrect error message in Json dropsection</t>
   </si>
+  <si>
+    <t>S01 in section number is accepted when it shouldn’t be</t>
+  </si>
 </sst>
 </file>
 
@@ -641,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -777,6 +780,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,6 +798,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="116">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1672,16 +1688,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2073,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A48" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2091,16 +2097,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -19919,14 +19925,31 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A57" s="43">
         <v>55</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="F57" s="40" t="str">
+      <c r="B57" s="24">
+        <v>5</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="40">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
+      </c>
+      <c r="G57" s="47">
+        <v>5</v>
+      </c>
+      <c r="H57" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -24583,124 +24606,129 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H2 H12:H21 H42:H48 H50:H1048576 H37:H40">
-    <cfRule type="containsText" dxfId="115" priority="40" operator="containsText" text="Stop current Development">
+  <conditionalFormatting sqref="H1:H2 H12:H21 H42:H48 H50:H56 H37:H40 H58:H1048576">
+    <cfRule type="containsText" dxfId="115" priority="41" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="114" priority="39" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="114" priority="40" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="113" priority="33" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="113" priority="34" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="112" priority="31" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="112" priority="32" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="111" priority="27" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="111" priority="28" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="110" priority="26" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="110" priority="27" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="109" priority="26" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="108" priority="21" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="108" priority="22" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="107" priority="20" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="107" priority="21" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="106" priority="19" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="106" priority="20" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="105" priority="18" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="105" priority="19" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="104" priority="16" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="104" priority="17" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="103" priority="13" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="103" priority="14" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="102" priority="13" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="101" priority="12" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="100" priority="10" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="100" priority="11" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="99" priority="10" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="98" priority="8" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="98" priority="9" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="97" priority="7" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="96" priority="7" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="95" priority="5" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="95" priority="6" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H36">
-    <cfRule type="containsText" dxfId="94" priority="4" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="94" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="containsText" dxfId="91" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
+      <formula>NOT(ISERROR(SEARCH("Stop current Development",H57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -24716,8 +24744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24734,16 +24762,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -26348,20 +26376,28 @@
       </c>
       <c r="B57" s="30">
         <f>'Our Bug Metrics'!B57</f>
-        <v>0</v>
-      </c>
-      <c r="C57" s="30">
+        <v>5</v>
+      </c>
+      <c r="C57" s="30" t="str">
         <f>'Our Bug Metrics'!C57</f>
-        <v>0</v>
-      </c>
-      <c r="D57" s="15">
+        <v>Bootstrap</v>
+      </c>
+      <c r="D57" s="15" t="str">
         <f>'Our Bug Metrics'!D57</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="11"/>
+        <v>S01 in section number is accepted when it shouldn’t be</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="12">
+        <v>43785</v>
+      </c>
+      <c r="G57" s="12">
+        <v>43785</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="58" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
@@ -35835,457 +35871,457 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="90" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="103" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="cellIs" dxfId="89" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="104" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5 E13:E20">
-    <cfRule type="containsBlanks" dxfId="88" priority="105">
+    <cfRule type="containsBlanks" dxfId="89" priority="105">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="88" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="86" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="89" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsBlanks" dxfId="85" priority="90">
+    <cfRule type="containsBlanks" dxfId="86" priority="90">
       <formula>LEN(TRIM(E10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="83" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="86" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsBlanks" dxfId="82" priority="87">
+    <cfRule type="containsBlanks" dxfId="83" priority="87">
       <formula>LEN(TRIM(E11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="80" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsBlanks" dxfId="79" priority="84">
+    <cfRule type="containsBlanks" dxfId="80" priority="84">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="80" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsBlanks" dxfId="76" priority="81">
+    <cfRule type="containsBlanks" dxfId="77" priority="81">
       <formula>LEN(TRIM(E8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="76" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="77" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsBlanks" dxfId="73" priority="78">
+    <cfRule type="containsBlanks" dxfId="74" priority="78">
       <formula>LEN(TRIM(E7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="70" priority="75">
+    <cfRule type="containsBlanks" dxfId="71" priority="75">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsBlanks" dxfId="67" priority="72">
+    <cfRule type="containsBlanks" dxfId="68" priority="72">
       <formula>LEN(TRIM(E6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="64" priority="69">
+    <cfRule type="containsBlanks" dxfId="65" priority="69">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="64" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="61" priority="66">
+    <cfRule type="containsBlanks" dxfId="62" priority="66">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="58" priority="63">
+    <cfRule type="containsBlanks" dxfId="59" priority="63">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="containsBlanks" dxfId="55" priority="60">
+    <cfRule type="containsBlanks" dxfId="56" priority="60">
       <formula>LEN(TRIM(E24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="containsBlanks" dxfId="52" priority="57">
+    <cfRule type="containsBlanks" dxfId="53" priority="57">
       <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsBlanks" dxfId="49" priority="54">
+    <cfRule type="containsBlanks" dxfId="50" priority="54">
       <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="containsBlanks" dxfId="46" priority="51">
+    <cfRule type="containsBlanks" dxfId="47" priority="51">
       <formula>LEN(TRIM(E28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="containsBlanks" dxfId="43" priority="48">
+    <cfRule type="containsBlanks" dxfId="44" priority="48">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="40" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="40" priority="42">
+    <cfRule type="containsBlanks" dxfId="41" priority="42">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsBlanks" dxfId="37" priority="39">
+    <cfRule type="containsBlanks" dxfId="38" priority="39">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsBlanks" dxfId="34" priority="36">
+    <cfRule type="containsBlanks" dxfId="35" priority="36">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E39">
-    <cfRule type="containsBlanks" dxfId="31" priority="33">
+    <cfRule type="containsBlanks" dxfId="32" priority="33">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsBlanks" dxfId="28" priority="30">
+    <cfRule type="containsBlanks" dxfId="29" priority="30">
       <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsBlanks" dxfId="25" priority="27">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
       <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E48">
-    <cfRule type="containsBlanks" dxfId="22" priority="24">
+    <cfRule type="containsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="containsBlanks" dxfId="19" priority="21">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
       <formula>LEN(TRIM(E49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(E53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(E54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(E55))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(E56))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E56" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E57" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36316,16 +36352,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -36373,7 +36409,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="51">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -36402,7 +36438,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36425,7 +36461,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="50"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -36448,7 +36484,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="50"/>
+      <c r="G6" s="51"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36471,7 +36507,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="51"/>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -36494,7 +36530,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="50"/>
+      <c r="G8" s="51"/>
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -36517,7 +36553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="50">
+      <c r="G9" s="51">
         <f>SUM(F9:F15)</f>
         <v>20</v>
       </c>
@@ -36546,7 +36582,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="51"/>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36569,7 +36605,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36592,7 +36628,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="50"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36615,7 +36651,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="50"/>
+      <c r="G13" s="51"/>
       <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36638,7 +36674,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="50"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36661,7 +36697,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="50"/>
+      <c r="G15" s="51"/>
       <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -36684,7 +36720,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="50">
+      <c r="G16" s="51">
         <f>SUM(F16:F19)</f>
         <v>20</v>
       </c>
@@ -36713,7 +36749,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="50"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36736,7 +36772,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="50"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36759,7 +36795,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="50"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -36782,7 +36818,7 @@
         <f>IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="51">
         <f>SUM(F20:F23)</f>
         <v>12</v>
       </c>
@@ -36810,7 +36846,7 @@
       <c r="F21" s="25">
         <v>5</v>
       </c>
-      <c r="G21" s="50"/>
+      <c r="G21" s="51"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36833,7 +36869,7 @@
         <f>IF($E22="Critical", 10, IF($E22="High",5, IF($E22="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G22" s="50"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -36856,7 +36892,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="50"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -41986,7 +42022,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated BM and Testcases.xlsx to show latest bugs
Updated BM and testcases.xlsx to show latest bugs

Co-Authored-By: serene98 <serene98@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Documents\GitHub\project-g5t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8F7D7D-49AE-4316-B938-E969C564FDFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C464D10A-4529-4EF9-9F92-D3F69FE19C8B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="167">
   <si>
     <t>Bug Log</t>
   </si>
@@ -530,6 +530,9 @@
   <si>
     <t>min_bid could not display correctly in round 2 active</t>
   </si>
+  <si>
+    <t>error message not out put correctly ie(invalid username\/password instead of invalid username, invalid password)</t>
+  </si>
 </sst>
 </file>
 
@@ -844,6 +847,16 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none"/>
       </fill>
@@ -903,16 +916,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2187,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView topLeftCell="A55" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20160,7 +20163,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" s="19" t="s">
         <v>64</v>
@@ -20187,7 +20190,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>64</v>
@@ -20241,7 +20244,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>64</v>
@@ -20271,13 +20274,13 @@
         <v>1</v>
       </c>
       <c r="G65" s="40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A66" s="43">
         <v>64</v>
       </c>
@@ -20301,7 +20304,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>64</v>
@@ -20331,20 +20334,37 @@
         <v>1</v>
       </c>
       <c r="G67" s="40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A68" s="43">
         <v>66</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="F68" s="40" t="str">
+      <c r="B68" s="24">
+        <v>5</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="E68" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" s="40">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G68" s="40">
+        <v>1</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -25029,8 +25049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2379E37-0698-4E89-97BA-D491A2AF9566}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26975,15 +26995,33 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="11"/>
+    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="30">
+        <f>'Our Bug Metrics'!$A68</f>
+        <v>66</v>
+      </c>
+      <c r="B68" s="8">
+        <v>6</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="13" t="str">
+        <f>'Our Bug Metrics'!D68</f>
+        <v>error message not out put correctly ie(invalid username\/password instead of invalid username, invalid password)</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="12">
+        <v>43786</v>
+      </c>
+      <c r="G68" s="12">
+        <v>43786</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
@@ -36761,52 +36799,52 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="containsBlanks" dxfId="6" priority="9">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(E65))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(E66))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="E67:E68">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="E67:E68">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+  <conditionalFormatting sqref="E67:E68">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(E67))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E67" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E68" xr:uid="{4D59F0F2-CE8D-4011-9D85-26CF084AD911}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>
@@ -42507,7 +42545,7 @@
     <mergeCell ref="G20:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>